<commit_message>
Update Use of Time Assessment.xlsx
</commit_message>
<xml_diff>
--- a/Management/Use of Time Assessment.xlsx
+++ b/Management/Use of Time Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacdw\Documents\Spring-2022\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC70558C-324A-46A1-8D52-0F748D9AA636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848671E1-AFB3-4D92-9F3F-3EB652369869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EB8D51B4-BFC4-40AB-B77E-F57530F23D28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="43">
   <si>
     <t xml:space="preserve">Sunday </t>
   </si>
@@ -156,13 +156,13 @@
     <t>Hang out w/ friends</t>
   </si>
   <si>
-    <t>eating</t>
-  </si>
-  <si>
     <t>Eat</t>
   </si>
   <si>
     <t>Class</t>
+  </si>
+  <si>
+    <t>Clean apartment</t>
   </si>
 </sst>
 </file>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7946A9D9-420C-4240-BBA7-78332F9B0AF1}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,6 +814,9 @@
       <c r="E9" t="s">
         <v>29</v>
       </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
       <c r="G9" t="s">
         <v>26</v>
       </c>
@@ -842,6 +845,9 @@
       </c>
       <c r="E10" t="s">
         <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
       </c>
       <c r="G10" t="s">
         <v>40</v>
@@ -869,6 +875,9 @@
       </c>
       <c r="E11" t="s">
         <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -895,6 +904,9 @@
       <c r="E12" t="s">
         <v>29</v>
       </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
       <c r="G12" t="s">
         <v>30</v>
       </c>
@@ -920,6 +932,9 @@
       <c r="E13" t="s">
         <v>29</v>
       </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
       <c r="G13" t="s">
         <v>30</v>
       </c>
@@ -945,6 +960,9 @@
       <c r="E14" t="s">
         <v>29</v>
       </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
       <c r="G14" t="s">
         <v>30</v>
       </c>
@@ -970,6 +988,9 @@
       <c r="E15" t="s">
         <v>29</v>
       </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
       <c r="G15" t="s">
         <v>30</v>
       </c>
@@ -995,6 +1016,9 @@
       <c r="E16" t="s">
         <v>29</v>
       </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
       <c r="G16" t="s">
         <v>30</v>
       </c>
@@ -1012,13 +1036,16 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
       </c>
       <c r="G17" t="s">
         <v>30</v>
@@ -1045,6 +1072,9 @@
       <c r="E18" t="s">
         <v>24</v>
       </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
       <c r="G18" t="s">
         <v>30</v>
       </c>
@@ -1155,7 +1185,7 @@
         <v>0.47222222222222199</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
         <v>27</v>
@@ -1183,7 +1213,7 @@
         <v>0.48611111111111099</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
@@ -1219,6 +1249,9 @@
       <c r="D24" t="s">
         <v>24</v>
       </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
       <c r="F24" t="s">
         <v>24</v>
       </c>
@@ -1244,6 +1277,12 @@
       <c r="D25" t="s">
         <v>24</v>
       </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
       <c r="G25" t="s">
         <v>24</v>
       </c>
@@ -1264,7 +1303,13 @@
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
       </c>
       <c r="J26" s="23"/>
       <c r="K26" s="6"/>
@@ -1283,7 +1328,13 @@
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
       </c>
       <c r="J27" s="23"/>
       <c r="K27" s="6"/>
@@ -1304,6 +1355,12 @@
       <c r="D28" t="s">
         <v>29</v>
       </c>
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
       <c r="J28" s="24"/>
       <c r="K28" s="10" t="s">
         <v>14</v>
@@ -1333,6 +1390,12 @@
       <c r="D29" t="s">
         <v>29</v>
       </c>
+      <c r="E29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17">
@@ -1347,6 +1410,12 @@
       <c r="D30" t="s">
         <v>29</v>
       </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
@@ -1361,6 +1430,12 @@
       <c r="D31" t="s">
         <v>29</v>
       </c>
+      <c r="E31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
       <c r="J31" s="3" t="s">
         <v>17</v>
       </c>
@@ -1381,6 +1456,12 @@
       <c r="D32" t="s">
         <v>29</v>
       </c>
+      <c r="E32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
       <c r="J32" s="13" t="s">
         <v>36</v>
       </c>
@@ -1399,6 +1480,12 @@
       <c r="D33" t="s">
         <v>29</v>
       </c>
+      <c r="E33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" t="s">
+        <v>29</v>
+      </c>
       <c r="J33" s="8" t="s">
         <v>25</v>
       </c>
@@ -1417,8 +1504,14 @@
       <c r="D34" t="s">
         <v>29</v>
       </c>
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" t="s">
+        <v>29</v>
+      </c>
       <c r="J34" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K34" s="8"/>
     </row>
@@ -1435,6 +1528,12 @@
       <c r="D35" t="s">
         <v>29</v>
       </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" t="s">
+        <v>29</v>
+      </c>
       <c r="J35" s="8" t="s">
         <v>37</v>
       </c>
@@ -1453,6 +1552,9 @@
       <c r="D36" t="s">
         <v>29</v>
       </c>
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
       <c r="F36" t="s">
         <v>30</v>
       </c>
@@ -1474,6 +1576,9 @@
       <c r="D37" t="s">
         <v>29</v>
       </c>
+      <c r="E37" t="s">
+        <v>29</v>
+      </c>
       <c r="F37" t="s">
         <v>30</v>
       </c>
@@ -1495,6 +1600,9 @@
       <c r="D38" t="s">
         <v>29</v>
       </c>
+      <c r="E38" t="s">
+        <v>29</v>
+      </c>
       <c r="F38" t="s">
         <v>30</v>
       </c>
@@ -1508,12 +1616,15 @@
         <v>0.70833333333333204</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
         <v>29</v>
       </c>
       <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" t="s">
         <v>29</v>
       </c>
       <c r="F39" t="s">
@@ -1529,19 +1640,22 @@
         <v>0.72222222222222099</v>
       </c>
       <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" t="s">
+        <v>30</v>
+      </c>
+      <c r="J40" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="C40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" t="s">
-        <v>30</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="K40" s="8"/>
     </row>
@@ -1641,7 +1755,7 @@
         <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D45" t="s">
         <v>24</v>
@@ -1650,7 +1764,7 @@
         <v>24</v>
       </c>
       <c r="F45" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
@@ -1663,7 +1777,7 @@
         <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D46" t="s">
         <v>31</v>
@@ -1672,7 +1786,7 @@
         <v>31</v>
       </c>
       <c r="F46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
@@ -1694,7 +1808,7 @@
         <v>31</v>
       </c>
       <c r="F47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
@@ -1716,7 +1830,7 @@
         <v>31</v>
       </c>
       <c r="F48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
@@ -1860,6 +1974,12 @@
       <c r="D55" t="s">
         <v>24</v>
       </c>
+      <c r="E55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
@@ -1874,6 +1994,12 @@
       <c r="D56" t="s">
         <v>24</v>
       </c>
+      <c r="E56" t="s">
+        <v>42</v>
+      </c>
+      <c r="F56" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
@@ -1886,7 +2012,13 @@
         <v>32</v>
       </c>
       <c r="D57" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="E57" t="s">
+        <v>42</v>
+      </c>
+      <c r="F57" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -1900,7 +2032,13 @@
         <v>32</v>
       </c>
       <c r="D58" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="E58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F58" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -1911,9 +2049,15 @@
         <v>33</v>
       </c>
       <c r="C59" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D59" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F59" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1930,6 +2074,12 @@
       <c r="D60" t="s">
         <v>29</v>
       </c>
+      <c r="E60" t="s">
+        <v>29</v>
+      </c>
+      <c r="F60" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
@@ -1944,6 +2094,12 @@
       <c r="D61" t="s">
         <v>29</v>
       </c>
+      <c r="E61" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="17">
@@ -1958,6 +2114,12 @@
       <c r="D62" t="s">
         <v>29</v>
       </c>
+      <c r="E62" t="s">
+        <v>29</v>
+      </c>
+      <c r="F62" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
@@ -1972,6 +2134,12 @@
       <c r="D63" t="s">
         <v>29</v>
       </c>
+      <c r="E63" t="s">
+        <v>29</v>
+      </c>
+      <c r="F63" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
@@ -1986,8 +2154,14 @@
       <c r="D64" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>29</v>
+      </c>
+      <c r="F64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
         <v>1.06944444444444</v>
       </c>
@@ -2000,13 +2174,19 @@
       <c r="D65" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <v>1.0833333333333299</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C66" t="s">
         <v>25</v>
@@ -2014,8 +2194,14 @@
       <c r="D66" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <v>1.0972222222222201</v>
       </c>
@@ -2028,8 +2214,14 @@
       <c r="D67" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
         <v>1.1111111111111101</v>
       </c>
@@ -2042,8 +2234,14 @@
       <c r="D68" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>25</v>
+      </c>
+      <c r="F68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>1.125</v>
       </c>
@@ -2056,8 +2254,14 @@
       <c r="D69" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>1.1388888888888899</v>
       </c>
@@ -2070,8 +2274,14 @@
       <c r="D70" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>25</v>
+      </c>
+      <c r="F70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
         <v>1.1527777777777699</v>
       </c>
@@ -2084,8 +2294,14 @@
       <c r="D71" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>25</v>
+      </c>
+      <c r="F71" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
         <v>1.1666666666666601</v>
       </c>
@@ -2098,8 +2314,14 @@
       <c r="D72" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>25</v>
+      </c>
+      <c r="F72" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <v>1.18055555555555</v>
       </c>
@@ -2112,8 +2334,14 @@
       <c r="D73" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>25</v>
+      </c>
+      <c r="F73" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
         <v>1.19444444444444</v>
       </c>
@@ -2126,8 +2354,14 @@
       <c r="D74" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>25</v>
+      </c>
+      <c r="F74" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
         <v>1.2083333333333299</v>
       </c>
@@ -2140,8 +2374,14 @@
       <c r="D75" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>25</v>
+      </c>
+      <c r="F75" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
         <v>1.2222222222222201</v>
       </c>
@@ -2154,8 +2394,14 @@
       <c r="D76" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="17">
         <v>1.2361111111111101</v>
       </c>
@@ -2168,8 +2414,14 @@
       <c r="D77" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>25</v>
+      </c>
+      <c r="F77" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="17">
         <v>1.25</v>
       </c>
@@ -2182,8 +2434,14 @@
       <c r="D78" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>25</v>
+      </c>
+      <c r="F78" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="17">
         <v>1.2638888888888899</v>
       </c>
@@ -2196,8 +2454,14 @@
       <c r="D79" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>25</v>
+      </c>
+      <c r="F79" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="17">
         <v>1.2777777777777699</v>
       </c>
@@ -2208,6 +2472,12 @@
         <v>25</v>
       </c>
       <c r="D80" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" t="s">
+        <v>25</v>
+      </c>
+      <c r="F80" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>